<commit_message>
added all files for the UFT commit
</commit_message>
<xml_diff>
--- a/Mobile_AOS/Default.xlsx
+++ b/Mobile_AOS/Default.xlsx
@@ -186,9 +186,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -199,7 +197,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -522,7 +522,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.5"/>
@@ -541,10 +541,10 @@
       </c>
     </row>
     <row>
-      <c s="3" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>